<commit_message>
commit 1052(Python) 1074 Reversing Linked List (25) 2018/8/11 17:06:09	部分正确	20	1074	Python (python 3)	24 ms
</commit_message>
<xml_diff>
--- a/PAT-Advanced-Level-Practice.xlsx
+++ b/PAT-Advanced-Level-Practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\hp_WJ\Documents\GitHub\PAT-Advanced-Level-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F883EE68-47D3-4975-9512-E7B81E88A76C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF0F9AB8-A208-41BE-8AF6-485AD084A7EA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9612" xr2:uid="{B69768DD-3D21-489D-9183-877BD9BED12D}"/>
   </bookViews>
@@ -937,8 +937,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1019,42 +1019,42 @@
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>1064</v>
+        <v>1003</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4">
-        <v>184</v>
+        <v>893</v>
       </c>
       <c r="E4" s="4">
-        <v>281</v>
+        <v>3592</v>
       </c>
       <c r="F4" s="4">
-        <v>0.65</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <v>1099</v>
+        <v>1004</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4">
         <v>30</v>
       </c>
       <c r="D5" s="4">
-        <v>144</v>
+        <v>680</v>
       </c>
       <c r="E5" s="4">
-        <v>221</v>
+        <v>1939</v>
       </c>
       <c r="F5" s="4">
-        <v>0.65</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1105,62 +1105,62 @@
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>1094</v>
+        <v>1007</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="C8" s="4">
         <v>25</v>
       </c>
       <c r="D8" s="4">
-        <v>168</v>
+        <v>649</v>
       </c>
       <c r="E8" s="4">
-        <v>266</v>
+        <v>3439</v>
       </c>
       <c r="F8" s="4">
-        <v>0.63</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
-        <v>1127</v>
+        <v>1009</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>132</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" s="4">
-        <v>133</v>
+        <v>746</v>
       </c>
       <c r="E9" s="4">
-        <v>233</v>
+        <v>2633</v>
       </c>
       <c r="F9" s="4">
-        <v>0.56999999999999995</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>1125</v>
+        <v>1010</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4">
         <v>25</v>
       </c>
       <c r="D10" s="4">
-        <v>95</v>
+        <v>546</v>
       </c>
       <c r="E10" s="4">
-        <v>170</v>
+        <v>5447</v>
       </c>
       <c r="F10" s="4">
-        <v>0.56000000000000005</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1211,42 +1211,42 @@
     </row>
     <row r="13" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
-        <v>1123</v>
+        <v>1013</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4">
-        <v>57</v>
+        <v>539</v>
       </c>
       <c r="E13" s="4">
-        <v>108</v>
+        <v>2038</v>
       </c>
       <c r="F13" s="4">
-        <v>0.53</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
-        <v>1102</v>
+        <v>1014</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
       <c r="C14" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D14" s="4">
-        <v>175</v>
+        <v>304</v>
       </c>
       <c r="E14" s="4">
-        <v>346</v>
+        <v>1335</v>
       </c>
       <c r="F14" s="4">
-        <v>0.51</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1274,102 +1274,102 @@
     </row>
     <row r="16" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>1083</v>
+        <v>1015</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D16" s="4">
-        <v>257</v>
+        <v>506</v>
       </c>
       <c r="E16" s="4">
-        <v>510</v>
+        <v>1794</v>
       </c>
       <c r="F16" s="4">
-        <v>0.5</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
-        <v>1134</v>
+        <v>1016</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4">
         <v>25</v>
       </c>
       <c r="D17" s="4">
-        <v>61</v>
+        <v>366</v>
       </c>
       <c r="E17" s="4">
-        <v>122</v>
+        <v>1742</v>
       </c>
       <c r="F17" s="4">
-        <v>0.5</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <v>1051</v>
+        <v>1017</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C18" s="4">
         <v>25</v>
       </c>
       <c r="D18" s="4">
-        <v>314</v>
+        <v>221</v>
       </c>
       <c r="E18" s="4">
-        <v>644</v>
+        <v>911</v>
       </c>
       <c r="F18" s="4">
-        <v>0.49</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
-        <v>1114</v>
+        <v>1018</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D19" s="4">
-        <v>91</v>
+        <v>218</v>
       </c>
       <c r="E19" s="4">
-        <v>187</v>
+        <v>1088</v>
       </c>
       <c r="F19" s="4">
-        <v>0.49</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
-        <v>1130</v>
+        <v>1019</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
       <c r="C20" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D20" s="4">
-        <v>61</v>
+        <v>576</v>
       </c>
       <c r="E20" s="4">
-        <v>125</v>
+        <v>1822</v>
       </c>
       <c r="F20" s="4">
-        <v>0.49</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1394,42 +1394,42 @@
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
-        <v>1030</v>
+        <v>1021</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C22" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D22" s="4">
-        <v>285</v>
+        <v>325</v>
       </c>
       <c r="E22" s="4">
-        <v>592</v>
+        <v>1254</v>
       </c>
       <c r="F22" s="4">
-        <v>0.48</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
-        <v>1056</v>
+        <v>1022</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="C23" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D23" s="4">
-        <v>219</v>
+        <v>300</v>
       </c>
       <c r="E23" s="4">
-        <v>453</v>
+        <v>1054</v>
       </c>
       <c r="F23" s="4">
-        <v>0.48</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1526,102 +1526,102 @@
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
-        <v>1086</v>
+        <v>1026</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="C28" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D28" s="4">
-        <v>202</v>
+        <v>119</v>
       </c>
       <c r="E28" s="4">
-        <v>424</v>
+        <v>675</v>
       </c>
       <c r="F28" s="4">
-        <v>0.48</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
-        <v>1092</v>
+        <v>1028</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="C29" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D29" s="4">
-        <v>201</v>
+        <v>392</v>
       </c>
       <c r="E29" s="4">
-        <v>423</v>
+        <v>1457</v>
       </c>
       <c r="F29" s="4">
-        <v>0.48</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
-        <v>1053</v>
+        <v>1029</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C30" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D30" s="4">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="E30" s="4">
-        <v>522</v>
+        <v>3255</v>
       </c>
       <c r="F30" s="4">
-        <v>0.46</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
-        <v>1054</v>
+        <v>1030</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C31" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D31" s="4">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E31" s="4">
-        <v>632</v>
+        <v>592</v>
       </c>
       <c r="F31" s="4">
-        <v>0.45</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
-        <v>1066</v>
+        <v>1031</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="C32" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D32" s="4">
-        <v>193</v>
+        <v>493</v>
       </c>
       <c r="E32" s="4">
-        <v>428</v>
+        <v>1448</v>
       </c>
       <c r="F32" s="4">
-        <v>0.45</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1649,339 +1649,339 @@
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
-        <v>1142</v>
+        <v>1033</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="C34" s="4">
         <v>25</v>
       </c>
       <c r="D34" s="4">
-        <v>88</v>
+        <v>231</v>
       </c>
       <c r="E34" s="4">
-        <v>199</v>
+        <v>799</v>
       </c>
       <c r="F34" s="4">
-        <v>0.44</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
-        <v>1084</v>
+        <v>1034</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C35" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D35" s="4">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="E35" s="4">
-        <v>604</v>
+        <v>981</v>
       </c>
       <c r="F35" s="4">
-        <v>0.43</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
-        <v>1087</v>
+        <v>1035</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="C36" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D36" s="4">
-        <v>157</v>
+        <v>416</v>
       </c>
       <c r="E36" s="4">
-        <v>364</v>
+        <v>1417</v>
       </c>
       <c r="F36" s="4">
-        <v>0.43</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
-        <v>1115</v>
+        <v>1036</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="C37" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D37" s="4">
-        <v>70</v>
+        <v>435</v>
       </c>
       <c r="E37" s="4">
-        <v>161</v>
+        <v>1077</v>
       </c>
       <c r="F37" s="4">
-        <v>0.43</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
-        <v>1146</v>
+        <v>1037</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>151</v>
+        <v>42</v>
       </c>
       <c r="C38" s="4">
         <v>25</v>
       </c>
       <c r="D38" s="4">
-        <v>144</v>
+        <v>322</v>
       </c>
       <c r="E38" s="4">
-        <v>334</v>
+        <v>879</v>
       </c>
       <c r="F38" s="4">
-        <v>0.43</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
-        <v>1045</v>
+        <v>1038</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C39" s="4">
         <v>30</v>
       </c>
       <c r="D39" s="4">
-        <v>172</v>
+        <v>254</v>
       </c>
       <c r="E39" s="4">
-        <v>424</v>
+        <v>789</v>
       </c>
       <c r="F39" s="4">
-        <v>0.41</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
-        <v>1106</v>
+        <v>1039</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="C40" s="4">
         <v>25</v>
       </c>
       <c r="D40" s="4">
-        <v>149</v>
+        <v>336</v>
       </c>
       <c r="E40" s="4">
-        <v>361</v>
+        <v>1492</v>
       </c>
       <c r="F40" s="4">
-        <v>0.41</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
-        <v>1122</v>
+        <v>1040</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="C41" s="4">
         <v>25</v>
       </c>
       <c r="D41" s="4">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="E41" s="4">
-        <v>140</v>
+        <v>728</v>
       </c>
       <c r="F41" s="4">
-        <v>0.41</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
-        <v>1124</v>
+        <v>1041</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>129</v>
+        <v>46</v>
       </c>
       <c r="C42" s="4">
         <v>20</v>
       </c>
       <c r="D42" s="4">
-        <v>78</v>
+        <v>375</v>
       </c>
       <c r="E42" s="4">
-        <v>191</v>
+        <v>971</v>
       </c>
       <c r="F42" s="4">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
-        <v>1036</v>
+        <v>1042</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C43" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D43" s="4">
-        <v>435</v>
+        <v>522</v>
       </c>
       <c r="E43" s="4">
-        <v>1077</v>
+        <v>1368</v>
       </c>
       <c r="F43" s="4">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
-        <v>1063</v>
+        <v>1043</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C44" s="4">
         <v>25</v>
       </c>
       <c r="D44" s="4">
-        <v>264</v>
+        <v>232</v>
       </c>
       <c r="E44" s="4">
-        <v>665</v>
+        <v>636</v>
       </c>
       <c r="F44" s="4">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="45" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
-        <v>1116</v>
+        <v>1044</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="C45" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D45" s="4">
-        <v>87</v>
+        <v>259</v>
       </c>
       <c r="E45" s="4">
-        <v>216</v>
+        <v>944</v>
       </c>
       <c r="F45" s="4">
-        <v>0.4</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C46" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D46" s="4">
-        <v>375</v>
+        <v>172</v>
       </c>
       <c r="E46" s="4">
-        <v>971</v>
+        <v>424</v>
       </c>
       <c r="F46" s="4">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
-        <v>1058</v>
+        <v>1046</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C47" s="4">
         <v>20</v>
       </c>
       <c r="D47" s="4">
-        <v>396</v>
+        <v>497</v>
       </c>
       <c r="E47" s="4">
-        <v>1008</v>
+        <v>1765</v>
       </c>
       <c r="F47" s="4">
-        <v>0.39</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
-        <v>1076</v>
+        <v>1047</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C48" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D48" s="4">
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="E48" s="4">
-        <v>490</v>
+        <v>1642</v>
       </c>
       <c r="F48" s="4">
-        <v>0.39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
-        <v>1079</v>
+        <v>1048</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C49" s="4">
         <v>25</v>
       </c>
       <c r="D49" s="4">
-        <v>177</v>
+        <v>477</v>
       </c>
       <c r="E49" s="4">
-        <v>457</v>
+        <v>1307</v>
       </c>
       <c r="F49" s="4">
-        <v>0.39</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
-        <v>1042</v>
+        <v>1049</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C50" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D50" s="4">
-        <v>522</v>
+        <v>200</v>
       </c>
       <c r="E50" s="4">
-        <v>1368</v>
+        <v>523</v>
       </c>
       <c r="F50" s="4">
         <v>0.38</v>
@@ -1989,62 +1989,65 @@
     </row>
     <row r="51" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C51" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D51" s="4">
-        <v>200</v>
+        <v>350</v>
       </c>
       <c r="E51" s="4">
-        <v>523</v>
+        <v>936</v>
       </c>
       <c r="F51" s="4">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
-        <v>1037</v>
+        <v>1051</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C52" s="4">
         <v>25</v>
       </c>
       <c r="D52" s="4">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E52" s="4">
-        <v>879</v>
+        <v>644</v>
       </c>
       <c r="F52" s="4">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C53" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D53" s="4">
-        <v>350</v>
+        <v>288</v>
       </c>
       <c r="E53" s="4">
-        <v>936</v>
+        <v>1307</v>
       </c>
       <c r="F53" s="4">
-        <v>0.37</v>
+        <v>0.22</v>
+      </c>
+      <c r="G53" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2072,250 +2075,250 @@
     </row>
     <row r="55" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
-        <v>1089</v>
+        <v>1053</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C55" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D55" s="4">
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="E55" s="4">
-        <v>446</v>
+        <v>522</v>
       </c>
       <c r="F55" s="4">
-        <v>0.37</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
-        <v>1109</v>
+        <v>1054</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C56" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D56" s="4">
-        <v>77</v>
+        <v>284</v>
       </c>
       <c r="E56" s="4">
-        <v>208</v>
+        <v>632</v>
       </c>
       <c r="F56" s="4">
-        <v>0.37</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
-        <v>1128</v>
+        <v>1055</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="C57" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D57" s="4">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E57" s="4">
-        <v>203</v>
+        <v>2508</v>
       </c>
       <c r="F57" s="4">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
-        <v>1043</v>
+        <v>1056</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C58" s="4">
         <v>25</v>
       </c>
       <c r="D58" s="4">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="E58" s="4">
-        <v>636</v>
+        <v>453</v>
       </c>
       <c r="F58" s="4">
-        <v>0.36</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
-        <v>1048</v>
+        <v>1057</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C59" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D59" s="4">
-        <v>477</v>
+        <v>163</v>
       </c>
       <c r="E59" s="4">
-        <v>1307</v>
+        <v>569</v>
       </c>
       <c r="F59" s="4">
-        <v>0.36</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
-        <v>1004</v>
+        <v>1058</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C60" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D60" s="4">
-        <v>680</v>
+        <v>396</v>
       </c>
       <c r="E60" s="4">
-        <v>1939</v>
+        <v>1008</v>
       </c>
       <c r="F60" s="4">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="61" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C61" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D61" s="4">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="E61" s="4">
-        <v>716</v>
+        <v>879</v>
       </c>
       <c r="F61" s="4">
-        <v>0.35</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
-        <v>1090</v>
+        <v>1060</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="C62" s="4">
         <v>25</v>
       </c>
       <c r="D62" s="4">
-        <v>161</v>
+        <v>260</v>
       </c>
       <c r="E62" s="4">
-        <v>464</v>
+        <v>1103</v>
       </c>
       <c r="F62" s="4">
-        <v>0.35</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
-        <v>1098</v>
+        <v>1061</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="C63" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D63" s="4">
-        <v>127</v>
+        <v>277</v>
       </c>
       <c r="E63" s="4">
-        <v>368</v>
+        <v>1212</v>
       </c>
       <c r="F63" s="4">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
-        <v>1107</v>
+        <v>1062</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="C64" s="4">
+        <v>25</v>
+      </c>
+      <c r="D64" s="4">
+        <v>330</v>
+      </c>
+      <c r="E64" s="4">
+        <v>993</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4">
+        <v>1063</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="4">
+        <v>25</v>
+      </c>
+      <c r="D65" s="4">
+        <v>264</v>
+      </c>
+      <c r="E65" s="4">
+        <v>665</v>
+      </c>
+      <c r="F65" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4">
+        <v>1064</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="4">
         <v>30</v>
       </c>
-      <c r="D64" s="4">
-        <v>146</v>
-      </c>
-      <c r="E64" s="4">
-        <v>419</v>
-      </c>
-      <c r="F64" s="4">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4">
-        <v>1121</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="4">
-        <v>25</v>
-      </c>
-      <c r="D65" s="4">
-        <v>85</v>
-      </c>
-      <c r="E65" s="4">
-        <v>242</v>
-      </c>
-      <c r="F65" s="4">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4">
-        <v>1031</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C66" s="4">
-        <v>20</v>
-      </c>
       <c r="D66" s="4">
-        <v>493</v>
+        <v>184</v>
       </c>
       <c r="E66" s="4">
-        <v>1448</v>
+        <v>281</v>
       </c>
       <c r="F66" s="4">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C67" s="4">
         <v>25</v>
@@ -2324,133 +2327,133 @@
         <v>193</v>
       </c>
       <c r="E67" s="4">
+        <v>428</v>
+      </c>
+      <c r="F67" s="4">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
+        <v>1067</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" s="4">
+        <v>25</v>
+      </c>
+      <c r="D68" s="4">
+        <v>250</v>
+      </c>
+      <c r="E68" s="4">
+        <v>858</v>
+      </c>
+      <c r="F68" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
+        <v>1068</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" s="4">
+        <v>30</v>
+      </c>
+      <c r="D69" s="4">
+        <v>118</v>
+      </c>
+      <c r="E69" s="4">
+        <v>415</v>
+      </c>
+      <c r="F69" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
+        <v>1069</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" s="4">
+        <v>20</v>
+      </c>
+      <c r="D70" s="4">
+        <v>252</v>
+      </c>
+      <c r="E70" s="4">
+        <v>716</v>
+      </c>
+      <c r="F70" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="4">
+        <v>1070</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" s="4">
+        <v>25</v>
+      </c>
+      <c r="D71" s="4">
+        <v>203</v>
+      </c>
+      <c r="E71" s="4">
+        <v>657</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
+        <v>1071</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="4">
+        <v>25</v>
+      </c>
+      <c r="D72" s="4">
+        <v>193</v>
+      </c>
+      <c r="E72" s="4">
         <v>561</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F72" s="4">
         <v>0.34</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4">
-        <v>1105</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" s="4">
-        <v>25</v>
-      </c>
-      <c r="D68" s="4">
-        <v>81</v>
-      </c>
-      <c r="E68" s="4">
-        <v>236</v>
-      </c>
-      <c r="F68" s="4">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="4">
-        <v>1062</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C69" s="4">
-        <v>25</v>
-      </c>
-      <c r="D69" s="4">
-        <v>330</v>
-      </c>
-      <c r="E69" s="4">
-        <v>993</v>
-      </c>
-      <c r="F69" s="4">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="4">
-        <v>1140</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C70" s="4">
-        <v>20</v>
-      </c>
-      <c r="D70" s="4">
-        <v>124</v>
-      </c>
-      <c r="E70" s="4">
-        <v>378</v>
-      </c>
-      <c r="F70" s="4">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="4">
-        <v>1019</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C71" s="4">
-        <v>20</v>
-      </c>
-      <c r="D71" s="4">
-        <v>576</v>
-      </c>
-      <c r="E71" s="4">
-        <v>1822</v>
-      </c>
-      <c r="F71" s="4">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="4">
-        <v>1038</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C72" s="4">
+    <row r="73" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <v>1072</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73" s="4">
         <v>30</v>
       </c>
-      <c r="D72" s="4">
-        <v>254</v>
-      </c>
-      <c r="E72" s="4">
-        <v>789</v>
-      </c>
-      <c r="F72" s="4">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="4">
-        <v>1059</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C73" s="4">
-        <v>25</v>
-      </c>
       <c r="D73" s="4">
-        <v>277</v>
+        <v>140</v>
       </c>
       <c r="E73" s="4">
-        <v>879</v>
+        <v>526</v>
       </c>
       <c r="F73" s="4">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>1073</v>
       </c>
@@ -2470,161 +2473,164 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
-        <v>1104</v>
+        <v>1074</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="C75" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D75" s="4">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="E75" s="4">
-        <v>696</v>
+        <v>748</v>
       </c>
       <c r="F75" s="4">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G75" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
-        <v>1129</v>
+        <v>1075</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="C76" s="4">
         <v>25</v>
       </c>
       <c r="D76" s="4">
-        <v>48</v>
+        <v>240</v>
       </c>
       <c r="E76" s="4">
-        <v>150</v>
+        <v>1294</v>
       </c>
       <c r="F76" s="4">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
-        <v>1132</v>
+        <v>1076</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="C77" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D77" s="4">
-        <v>103</v>
+        <v>193</v>
       </c>
       <c r="E77" s="4">
-        <v>326</v>
+        <v>490</v>
       </c>
       <c r="F77" s="4">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
-        <v>1070</v>
+        <v>1077</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C78" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D78" s="4">
-        <v>203</v>
+        <v>341</v>
       </c>
       <c r="E78" s="4">
-        <v>657</v>
+        <v>1927</v>
       </c>
       <c r="F78" s="4">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C79" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D79" s="4">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E79" s="4">
-        <v>735</v>
+        <v>886</v>
       </c>
       <c r="F79" s="4">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
-        <v>1088</v>
+        <v>1079</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C80" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D80" s="4">
         <v>177</v>
       </c>
       <c r="E80" s="4">
-        <v>565</v>
+        <v>457</v>
       </c>
       <c r="F80" s="4">
-        <v>0.31</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
-        <v>1093</v>
+        <v>1080</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C81" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D81" s="4">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="E81" s="4">
-        <v>695</v>
+        <v>1099</v>
       </c>
       <c r="F81" s="4">
-        <v>0.31</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
-        <v>1103</v>
+        <v>1081</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C82" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D82" s="4">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="E82" s="4">
-        <v>814</v>
+        <v>735</v>
       </c>
       <c r="F82" s="4">
         <v>0.31</v>
@@ -2632,482 +2638,482 @@
     </row>
     <row r="83" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C83" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D83" s="4">
-        <v>192</v>
+        <v>230</v>
       </c>
       <c r="E83" s="4">
-        <v>649</v>
+        <v>856</v>
       </c>
       <c r="F83" s="4">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
-        <v>1097</v>
+        <v>1083</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C84" s="4">
         <v>25</v>
       </c>
       <c r="D84" s="4">
-        <v>177</v>
+        <v>257</v>
       </c>
       <c r="E84" s="4">
-        <v>585</v>
+        <v>510</v>
       </c>
       <c r="F84" s="4">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
-        <v>1100</v>
+        <v>1084</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C85" s="4">
         <v>20</v>
       </c>
       <c r="D85" s="4">
-        <v>186</v>
+        <v>257</v>
       </c>
       <c r="E85" s="4">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="F85" s="4">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
-        <v>1133</v>
+        <v>1085</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="C86" s="4">
         <v>25</v>
       </c>
       <c r="D86" s="4">
-        <v>62</v>
+        <v>369</v>
       </c>
       <c r="E86" s="4">
-        <v>205</v>
+        <v>1406</v>
       </c>
       <c r="F86" s="4">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
-        <v>1033</v>
+        <v>1086</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="C87" s="4">
         <v>25</v>
       </c>
       <c r="D87" s="4">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="E87" s="4">
-        <v>799</v>
+        <v>424</v>
       </c>
       <c r="F87" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
-        <v>1034</v>
+        <v>1087</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="C88" s="4">
         <v>30</v>
       </c>
       <c r="D88" s="4">
-        <v>281</v>
+        <v>157</v>
       </c>
       <c r="E88" s="4">
-        <v>981</v>
+        <v>364</v>
       </c>
       <c r="F88" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
-        <v>1035</v>
+        <v>1088</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="C89" s="4">
         <v>20</v>
       </c>
       <c r="D89" s="4">
-        <v>416</v>
+        <v>177</v>
       </c>
       <c r="E89" s="4">
-        <v>1417</v>
+        <v>565</v>
       </c>
       <c r="F89" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
-        <v>1057</v>
+        <v>1089</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C90" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D90" s="4">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E90" s="4">
-        <v>569</v>
+        <v>446</v>
       </c>
       <c r="F90" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
-        <v>1067</v>
+        <v>1090</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C91" s="4">
         <v>25</v>
       </c>
       <c r="D91" s="4">
-        <v>250</v>
+        <v>161</v>
       </c>
       <c r="E91" s="4">
-        <v>858</v>
+        <v>464</v>
       </c>
       <c r="F91" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
-        <v>1110</v>
+        <v>1091</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C92" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D92" s="4">
-        <v>78</v>
+        <v>164</v>
       </c>
       <c r="E92" s="4">
-        <v>273</v>
+        <v>593</v>
       </c>
       <c r="F92" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
-        <v>1136</v>
+        <v>1092</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="C93" s="4">
         <v>20</v>
       </c>
       <c r="D93" s="4">
-        <v>80</v>
+        <v>201</v>
       </c>
       <c r="E93" s="4">
-        <v>276</v>
+        <v>423</v>
       </c>
       <c r="F93" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="94" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
-        <v>1147</v>
+        <v>1093</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
       <c r="C94" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D94" s="4">
-        <v>119</v>
+        <v>213</v>
       </c>
       <c r="E94" s="4">
-        <v>412</v>
+        <v>695</v>
       </c>
       <c r="F94" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
-        <v>1009</v>
+        <v>1094</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="C95" s="4">
         <v>25</v>
       </c>
       <c r="D95" s="4">
-        <v>746</v>
+        <v>168</v>
       </c>
       <c r="E95" s="4">
-        <v>2633</v>
+        <v>266</v>
       </c>
       <c r="F95" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
-        <v>1015</v>
+        <v>1095</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C96" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D96" s="4">
-        <v>506</v>
+        <v>146</v>
       </c>
       <c r="E96" s="4">
-        <v>1794</v>
+        <v>747</v>
       </c>
       <c r="F96" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
-        <v>1022</v>
+        <v>1096</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="C97" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D97" s="4">
-        <v>300</v>
+        <v>192</v>
       </c>
       <c r="E97" s="4">
-        <v>1054</v>
+        <v>649</v>
       </c>
       <c r="F97" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="98" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
-        <v>1046</v>
+        <v>1097</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="C98" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D98" s="4">
-        <v>497</v>
+        <v>177</v>
       </c>
       <c r="E98" s="4">
-        <v>1765</v>
+        <v>585</v>
       </c>
       <c r="F98" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
-        <v>1068</v>
+        <v>1098</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="C99" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D99" s="4">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="E99" s="4">
-        <v>415</v>
+        <v>368</v>
       </c>
       <c r="F99" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
-        <v>1074</v>
+        <v>1099</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="C100" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D100" s="4">
-        <v>207</v>
+        <v>144</v>
       </c>
       <c r="E100" s="4">
-        <v>748</v>
+        <v>221</v>
       </c>
       <c r="F100" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="101" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
-        <v>1091</v>
+        <v>1100</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C101" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D101" s="4">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="E101" s="4">
-        <v>593</v>
+        <v>617</v>
       </c>
       <c r="F101" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="102" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
-        <v>1118</v>
+        <v>1101</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C102" s="4">
         <v>25</v>
       </c>
       <c r="D102" s="4">
-        <v>70</v>
+        <v>194</v>
       </c>
       <c r="E102" s="4">
-        <v>248</v>
+        <v>792</v>
       </c>
       <c r="F102" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="103" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
-        <v>1028</v>
+        <v>1102</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="C103" s="4">
         <v>25</v>
       </c>
       <c r="D103" s="4">
-        <v>392</v>
+        <v>175</v>
       </c>
       <c r="E103" s="4">
-        <v>1457</v>
+        <v>346</v>
       </c>
       <c r="F103" s="4">
-        <v>0.27</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
-        <v>1044</v>
+        <v>1103</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="C104" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D104" s="4">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E104" s="4">
-        <v>944</v>
+        <v>814</v>
       </c>
       <c r="F104" s="4">
-        <v>0.27</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
-        <v>1072</v>
+        <v>1104</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="C105" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D105" s="4">
-        <v>140</v>
+        <v>225</v>
       </c>
       <c r="E105" s="4">
-        <v>526</v>
+        <v>696</v>
       </c>
       <c r="F105" s="4">
-        <v>0.27</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="106" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
-        <v>1082</v>
+        <v>1105</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="C106" s="4">
         <v>25</v>
       </c>
       <c r="D106" s="4">
-        <v>230</v>
+        <v>81</v>
       </c>
       <c r="E106" s="4">
-        <v>856</v>
+        <v>236</v>
       </c>
       <c r="F106" s="4">
-        <v>0.27</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3135,59 +3141,59 @@
     </row>
     <row r="108" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C108" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D108" s="4">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="E108" s="4">
-        <v>340</v>
+        <v>361</v>
       </c>
       <c r="F108" s="4">
-        <v>0.27</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
-        <v>1117</v>
+        <v>1107</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C109" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D109" s="4">
-        <v>80</v>
+        <v>146</v>
       </c>
       <c r="E109" s="4">
-        <v>293</v>
+        <v>419</v>
       </c>
       <c r="F109" s="4">
-        <v>0.27</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
-        <v>1137</v>
+        <v>1108</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C110" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D110" s="4">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E110" s="4">
-        <v>297</v>
+        <v>340</v>
       </c>
       <c r="F110" s="4">
         <v>0.27</v>
@@ -3195,142 +3201,142 @@
     </row>
     <row r="111" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
-        <v>1013</v>
+        <v>1109</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="C111" s="4">
         <v>25</v>
       </c>
       <c r="D111" s="4">
-        <v>539</v>
+        <v>77</v>
       </c>
       <c r="E111" s="4">
-        <v>2038</v>
+        <v>208</v>
       </c>
       <c r="F111" s="4">
-        <v>0.26</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
-        <v>1021</v>
+        <v>1110</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="C112" s="4">
         <v>25</v>
       </c>
       <c r="D112" s="4">
-        <v>325</v>
+        <v>78</v>
       </c>
       <c r="E112" s="4">
-        <v>1254</v>
+        <v>273</v>
       </c>
       <c r="F112" s="4">
-        <v>0.26</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="113" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
-        <v>1040</v>
+        <v>1111</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="C113" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D113" s="4">
-        <v>188</v>
+        <v>64</v>
       </c>
       <c r="E113" s="4">
-        <v>728</v>
+        <v>275</v>
       </c>
       <c r="F113" s="4">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
-        <v>1078</v>
+        <v>1112</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="C114" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D114" s="4">
-        <v>227</v>
+        <v>82</v>
       </c>
       <c r="E114" s="4">
-        <v>886</v>
+        <v>333</v>
       </c>
       <c r="F114" s="4">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
-        <v>1085</v>
+        <v>1114</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="C115" s="4">
         <v>25</v>
       </c>
       <c r="D115" s="4">
-        <v>369</v>
+        <v>91</v>
       </c>
       <c r="E115" s="4">
-        <v>1406</v>
+        <v>187</v>
       </c>
       <c r="F115" s="4">
-        <v>0.26</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="116" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
-        <v>1138</v>
+        <v>1115</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="C116" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D116" s="4">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E116" s="4">
-        <v>315</v>
+        <v>161</v>
       </c>
       <c r="F116" s="4">
-        <v>0.26</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="117" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
-        <v>1003</v>
+        <v>1116</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="C117" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D117" s="4">
-        <v>893</v>
+        <v>87</v>
       </c>
       <c r="E117" s="4">
-        <v>3592</v>
+        <v>216</v>
       </c>
       <c r="F117" s="4">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="118" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3358,279 +3364,279 @@
     </row>
     <row r="119" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4">
-        <v>1112</v>
+        <v>1117</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C119" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D119" s="4">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E119" s="4">
-        <v>333</v>
+        <v>293</v>
       </c>
       <c r="F119" s="4">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="120" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
-        <v>1135</v>
+        <v>1118</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C120" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D120" s="4">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E120" s="4">
-        <v>185</v>
+        <v>248</v>
       </c>
       <c r="F120" s="4">
-        <v>0.25</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="121" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
-        <v>1017</v>
+        <v>1119</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C121" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D121" s="4">
-        <v>221</v>
+        <v>57</v>
       </c>
       <c r="E121" s="4">
-        <v>911</v>
+        <v>370</v>
       </c>
       <c r="F121" s="4">
-        <v>0.24</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="122" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4">
-        <v>1060</v>
+        <v>1121</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="C122" s="4">
         <v>25</v>
       </c>
       <c r="D122" s="4">
-        <v>260</v>
+        <v>85</v>
       </c>
       <c r="E122" s="4">
-        <v>1103</v>
+        <v>242</v>
       </c>
       <c r="F122" s="4">
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="123" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
-        <v>1101</v>
+        <v>1122</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C123" s="4">
         <v>25</v>
       </c>
       <c r="D123" s="4">
-        <v>194</v>
+        <v>58</v>
       </c>
       <c r="E123" s="4">
-        <v>792</v>
+        <v>140</v>
       </c>
       <c r="F123" s="4">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="124" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C124" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D124" s="4">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E124" s="4">
-        <v>221</v>
+        <v>108</v>
       </c>
       <c r="F124" s="4">
-        <v>0.24</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="125" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4">
-        <v>1143</v>
+        <v>1124</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="C125" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D125" s="4">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E125" s="4">
-        <v>335</v>
+        <v>191</v>
       </c>
       <c r="F125" s="4">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="126" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4">
-        <v>1145</v>
+        <v>1125</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C126" s="4">
         <v>25</v>
       </c>
       <c r="D126" s="4">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E126" s="4">
-        <v>460</v>
+        <v>170</v>
       </c>
       <c r="F126" s="4">
-        <v>0.24</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="127" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="4">
-        <v>1014</v>
+        <v>1126</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="C127" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D127" s="4">
-        <v>304</v>
+        <v>53</v>
       </c>
       <c r="E127" s="4">
-        <v>1335</v>
+        <v>221</v>
       </c>
       <c r="F127" s="4">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="128" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="4">
-        <v>1039</v>
+        <v>1127</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="C128" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D128" s="4">
-        <v>336</v>
+        <v>133</v>
       </c>
       <c r="E128" s="4">
-        <v>1492</v>
+        <v>233</v>
       </c>
       <c r="F128" s="4">
-        <v>0.23</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="129" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
-        <v>1061</v>
+        <v>1128</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="C129" s="4">
         <v>20</v>
       </c>
       <c r="D129" s="4">
-        <v>277</v>
+        <v>76</v>
       </c>
       <c r="E129" s="4">
-        <v>1212</v>
+        <v>203</v>
       </c>
       <c r="F129" s="4">
-        <v>0.23</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="130" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="4">
-        <v>1111</v>
+        <v>1129</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="C130" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D130" s="4">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E130" s="4">
-        <v>275</v>
+        <v>150</v>
       </c>
       <c r="F130" s="4">
-        <v>0.23</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="131" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
-        <v>1144</v>
+        <v>1130</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C131" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D131" s="4">
-        <v>229</v>
+        <v>61</v>
       </c>
       <c r="E131" s="4">
-        <v>982</v>
+        <v>125</v>
       </c>
       <c r="F131" s="4">
-        <v>0.23</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="132" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
-        <v>1052</v>
+        <v>1131</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="C132" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D132" s="4">
-        <v>288</v>
+        <v>60</v>
       </c>
       <c r="E132" s="4">
-        <v>1307</v>
+        <v>276</v>
       </c>
       <c r="F132" s="4">
         <v>0.22</v>
@@ -3638,182 +3644,182 @@
     </row>
     <row r="133" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
-        <v>1080</v>
+        <v>1132</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="C133" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D133" s="4">
-        <v>240</v>
+        <v>103</v>
       </c>
       <c r="E133" s="4">
-        <v>1099</v>
+        <v>326</v>
       </c>
       <c r="F133" s="4">
-        <v>0.22</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="134" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C134" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D134" s="4">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E134" s="4">
-        <v>276</v>
+        <v>205</v>
       </c>
       <c r="F134" s="4">
-        <v>0.22</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="135" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
-        <v>1016</v>
+        <v>1134</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="C135" s="4">
         <v>25</v>
       </c>
       <c r="D135" s="4">
-        <v>366</v>
+        <v>61</v>
       </c>
       <c r="E135" s="4">
-        <v>1742</v>
+        <v>122</v>
       </c>
       <c r="F135" s="4">
-        <v>0.21</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="136" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4">
-        <v>1018</v>
+        <v>1135</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>23</v>
+        <v>140</v>
       </c>
       <c r="C136" s="4">
         <v>30</v>
       </c>
       <c r="D136" s="4">
-        <v>218</v>
+        <v>47</v>
       </c>
       <c r="E136" s="4">
-        <v>1088</v>
+        <v>185</v>
       </c>
       <c r="F136" s="4">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="137" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="4">
-        <v>1095</v>
+        <v>1136</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="C137" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D137" s="4">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="E137" s="4">
-        <v>747</v>
+        <v>276</v>
       </c>
       <c r="F137" s="4">
-        <v>0.2</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="138" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4">
-        <v>1007</v>
+        <v>1137</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="C138" s="4">
         <v>25</v>
       </c>
       <c r="D138" s="4">
-        <v>649</v>
+        <v>79</v>
       </c>
       <c r="E138" s="4">
-        <v>3439</v>
+        <v>297</v>
       </c>
       <c r="F138" s="4">
-        <v>0.19</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="139" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="4">
-        <v>1075</v>
+        <v>1138</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="C139" s="4">
         <v>25</v>
       </c>
       <c r="D139" s="4">
-        <v>240</v>
+        <v>82</v>
       </c>
       <c r="E139" s="4">
-        <v>1294</v>
+        <v>315</v>
       </c>
       <c r="F139" s="4">
-        <v>0.19</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="140" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="4">
-        <v>1026</v>
+        <v>1139</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>31</v>
+        <v>144</v>
       </c>
       <c r="C140" s="4">
         <v>30</v>
       </c>
       <c r="D140" s="4">
-        <v>119</v>
+        <v>60</v>
       </c>
       <c r="E140" s="4">
-        <v>675</v>
+        <v>386</v>
       </c>
       <c r="F140" s="4">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="141" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="4">
-        <v>1077</v>
+        <v>1140</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="C141" s="4">
         <v>20</v>
       </c>
       <c r="D141" s="4">
-        <v>341</v>
+        <v>124</v>
       </c>
       <c r="E141" s="4">
-        <v>1927</v>
+        <v>378</v>
       </c>
       <c r="F141" s="4">
-        <v>0.18</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="142" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3838,122 +3844,122 @@
     </row>
     <row r="143" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="4">
-        <v>1139</v>
+        <v>1142</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C143" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D143" s="4">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="E143" s="4">
-        <v>386</v>
+        <v>199</v>
       </c>
       <c r="F143" s="4">
-        <v>0.16</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="144" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="4">
-        <v>1119</v>
+        <v>1143</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="C144" s="4">
         <v>30</v>
       </c>
       <c r="D144" s="4">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E144" s="4">
-        <v>370</v>
+        <v>335</v>
       </c>
       <c r="F144" s="4">
-        <v>0.15</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="145" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
-        <v>1010</v>
+        <v>1144</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="C145" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D145" s="4">
-        <v>546</v>
+        <v>229</v>
       </c>
       <c r="E145" s="4">
-        <v>5447</v>
+        <v>982</v>
       </c>
       <c r="F145" s="4">
-        <v>0.1</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="146" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
-        <v>1029</v>
+        <v>1145</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="C146" s="4">
         <v>25</v>
       </c>
       <c r="D146" s="4">
-        <v>207</v>
+        <v>112</v>
       </c>
       <c r="E146" s="4">
-        <v>3255</v>
+        <v>460</v>
       </c>
       <c r="F146" s="4">
-        <v>0.06</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="147" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
-        <v>1047</v>
+        <v>1146</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="C147" s="4">
         <v>25</v>
       </c>
       <c r="D147" s="4">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="E147" s="4">
-        <v>1642</v>
+        <v>334</v>
       </c>
       <c r="F147" s="4">
-        <v>0</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="148" spans="1:6" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="4">
-        <v>1055</v>
+        <v>1147</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="C148" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D148" s="4">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="E148" s="4">
-        <v>2508</v>
+        <v>412</v>
       </c>
       <c r="F148" s="4">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -3962,158 +3968,158 @@
       <filters blank="1"/>
     </filterColumn>
     <sortState ref="A4:G148">
-      <sortCondition descending="1" ref="F1:F148"/>
+      <sortCondition ref="A1:A148"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805528788582400" xr:uid="{82B400A0-499F-47C9-8D89-545D1A3E2C92}"/>
     <hyperlink ref="B3" r:id="rId2" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805526272000000" xr:uid="{408FA3D8-322D-4D7B-BC31-E8665E08E7C7}"/>
-    <hyperlink ref="B117" r:id="rId3" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805523835109376" xr:uid="{1EAE05E0-A1DD-4229-8B3D-E40A4214A098}"/>
-    <hyperlink ref="B60" r:id="rId4" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805521431773184" xr:uid="{B7D987CC-3EA0-4961-87BF-5ABC20B1EB90}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805523835109376" xr:uid="{1EAE05E0-A1DD-4229-8B3D-E40A4214A098}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805521431773184" xr:uid="{B7D987CC-3EA0-4961-87BF-5ABC20B1EB90}"/>
     <hyperlink ref="B6" r:id="rId5" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805519074574336" xr:uid="{BD29C8C9-1871-434A-939C-484E21C513B4}"/>
     <hyperlink ref="B7" r:id="rId6" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805516654460928" xr:uid="{B6AE5B69-D15D-401A-B9FF-CC13C1DB0297}"/>
-    <hyperlink ref="B138" r:id="rId7" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805514284679168" xr:uid="{CB0A8259-AD16-478B-A80C-8C51750A057C}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805514284679168" xr:uid="{CB0A8259-AD16-478B-A80C-8C51750A057C}"/>
     <hyperlink ref="B11" r:id="rId8" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805511923286016" xr:uid="{C0CF408D-AC5D-4383-854C-DB8F054B46D8}"/>
-    <hyperlink ref="B95" r:id="rId9" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805509540921344" xr:uid="{6FABFB40-FC0A-4067-BE0B-D2BC8F8DCB98}"/>
-    <hyperlink ref="B145" r:id="rId10" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805507225665536" xr:uid="{5EECE5EC-52C9-47F3-9AE1-ACEE97A98AB1}"/>
+    <hyperlink ref="B9" r:id="rId9" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805509540921344" xr:uid="{6FABFB40-FC0A-4067-BE0B-D2BC8F8DCB98}"/>
+    <hyperlink ref="B10" r:id="rId10" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805507225665536" xr:uid="{5EECE5EC-52C9-47F3-9AE1-ACEE97A98AB1}"/>
     <hyperlink ref="B12" r:id="rId11" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805504927186944" xr:uid="{E474FD39-9F00-4A4B-8B6C-2818E1A62314}"/>
     <hyperlink ref="B15" r:id="rId12" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805502658068480" xr:uid="{3879AB51-3071-4C1A-A563-987B24575425}"/>
-    <hyperlink ref="B111" r:id="rId13" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805500414115840" xr:uid="{92E069AC-EA6D-45F1-B446-AB92259BB93C}"/>
-    <hyperlink ref="B127" r:id="rId14" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805498207911936" xr:uid="{B59AAAB5-5C44-43AF-B6A6-CB3852BD5B0D}"/>
-    <hyperlink ref="B96" r:id="rId15" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805495863296000" xr:uid="{63CCE55A-9030-48FA-8526-499E8288A3DF}"/>
-    <hyperlink ref="B135" r:id="rId16" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805493648703488" xr:uid="{7FA151F4-6C20-44A7-9AC6-546673A9D18E}"/>
-    <hyperlink ref="B121" r:id="rId17" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805491530579968" xr:uid="{FADC2D3A-2950-4112-B945-E92FE6076DC8}"/>
-    <hyperlink ref="B136" r:id="rId18" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805489282433024" xr:uid="{8DAC45D6-792A-423A-ACD6-B0A57AEF423C}"/>
-    <hyperlink ref="B71" r:id="rId19" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805487143337984" xr:uid="{2E267083-0CC2-4CAA-9896-2E36003DCE20}"/>
+    <hyperlink ref="B13" r:id="rId13" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805500414115840" xr:uid="{92E069AC-EA6D-45F1-B446-AB92259BB93C}"/>
+    <hyperlink ref="B14" r:id="rId14" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805498207911936" xr:uid="{B59AAAB5-5C44-43AF-B6A6-CB3852BD5B0D}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805495863296000" xr:uid="{63CCE55A-9030-48FA-8526-499E8288A3DF}"/>
+    <hyperlink ref="B17" r:id="rId16" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805493648703488" xr:uid="{7FA151F4-6C20-44A7-9AC6-546673A9D18E}"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805491530579968" xr:uid="{FADC2D3A-2950-4112-B945-E92FE6076DC8}"/>
+    <hyperlink ref="B19" r:id="rId18" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805489282433024" xr:uid="{8DAC45D6-792A-423A-ACD6-B0A57AEF423C}"/>
+    <hyperlink ref="B20" r:id="rId19" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805487143337984" xr:uid="{2E267083-0CC2-4CAA-9896-2E36003DCE20}"/>
     <hyperlink ref="B21" r:id="rId20" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805485033603072" xr:uid="{4825B473-F6A2-476F-B32E-3354244E7EDC}"/>
-    <hyperlink ref="B112" r:id="rId21" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805482919673856" xr:uid="{BCB4A002-2E32-42BB-8FC3-622F707ABC5E}"/>
-    <hyperlink ref="B97" r:id="rId22" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805480801550336" xr:uid="{79FE4C9E-20AC-466E-A2B2-710CEE0C0CD7}"/>
+    <hyperlink ref="B22" r:id="rId21" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805482919673856" xr:uid="{BCB4A002-2E32-42BB-8FC3-622F707ABC5E}"/>
+    <hyperlink ref="B23" r:id="rId22" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805480801550336" xr:uid="{79FE4C9E-20AC-466E-A2B2-710CEE0C0CD7}"/>
     <hyperlink ref="B24" r:id="rId23" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805478658260992" xr:uid="{9D0B6792-97F5-4E53-AB5E-FEB5AB61C633}"/>
     <hyperlink ref="B25" r:id="rId24" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805476473028608" xr:uid="{63522518-6918-4BF2-B7ED-3D220EB50906}"/>
     <hyperlink ref="B27" r:id="rId25" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805474338127872" xr:uid="{5EE2328B-01EE-4A94-8272-BB2024DCBCD6}"/>
-    <hyperlink ref="B140" r:id="rId26" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805472333250560" xr:uid="{418FB35D-E9A1-405B-8456-1E22867147A9}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805472333250560" xr:uid="{418FB35D-E9A1-405B-8456-1E22867147A9}"/>
     <hyperlink ref="B26" r:id="rId27" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805470349344768" xr:uid="{E5447B5C-4BF9-45DB-BFCD-A774CD02682C}"/>
-    <hyperlink ref="B103" r:id="rId28" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805468327690240" xr:uid="{2AA84E71-DDF5-45A0-80CF-B7C4A770732C}"/>
-    <hyperlink ref="B146" r:id="rId29" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805466364755968" xr:uid="{0BD2CDCE-0BA4-462F-A164-1ABB39F3B993}"/>
-    <hyperlink ref="B22" r:id="rId30" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805464397627392" xr:uid="{358377DA-8DC0-4701-89B2-1268214BDAAA}"/>
-    <hyperlink ref="B66" r:id="rId31" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805462535356416" xr:uid="{EE83739C-0F34-4373-94DC-C27F76CE323C}"/>
+    <hyperlink ref="B29" r:id="rId28" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805468327690240" xr:uid="{2AA84E71-DDF5-45A0-80CF-B7C4A770732C}"/>
+    <hyperlink ref="B30" r:id="rId29" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805466364755968" xr:uid="{0BD2CDCE-0BA4-462F-A164-1ABB39F3B993}"/>
+    <hyperlink ref="B31" r:id="rId30" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805464397627392" xr:uid="{358377DA-8DC0-4701-89B2-1268214BDAAA}"/>
+    <hyperlink ref="B32" r:id="rId31" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805462535356416" xr:uid="{EE83739C-0F34-4373-94DC-C27F76CE323C}"/>
     <hyperlink ref="B33" r:id="rId32" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805460652113920" xr:uid="{6436A962-F078-4578-8BAA-2C26EFA6025A}"/>
-    <hyperlink ref="B87" r:id="rId33" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805458722734080" xr:uid="{9FE3426B-EE65-4BD4-82D5-4353808187B3}"/>
-    <hyperlink ref="B88" r:id="rId34" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805456881434624" xr:uid="{0BD5DC6A-5CF6-4859-BBDF-28DEE169D65C}"/>
-    <hyperlink ref="B89" r:id="rId35" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805454989803520" xr:uid="{3EF6CF64-9BE5-485E-915C-11254311497B}"/>
-    <hyperlink ref="B43" r:id="rId36" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805453203030016" xr:uid="{CEC48129-09DA-4BCD-8D86-EF37E2C8B021}"/>
-    <hyperlink ref="B52" r:id="rId37" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805451374313472" xr:uid="{8C7877FB-C53F-4C82-B693-8F3919AB588E}"/>
-    <hyperlink ref="B72" r:id="rId38" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805449625288704" xr:uid="{4C40021A-4B5F-49D8-953B-7B8BC23ACCE9}"/>
-    <hyperlink ref="B128" r:id="rId39" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805447855292416" xr:uid="{C07F5AB7-5FB1-4864-8D22-202836B5B8ED}"/>
-    <hyperlink ref="B113" r:id="rId40" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805446102073344" xr:uid="{A9A7264A-747F-48AE-82D8-302D31B349A1}"/>
-    <hyperlink ref="B46" r:id="rId41" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805444361437184" xr:uid="{3D1A5343-7724-4C55-AA9D-522F36978383}"/>
-    <hyperlink ref="B50" r:id="rId42" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805442671132672" xr:uid="{30B7B1A6-B7DF-41C8-A7FA-F624ABB35544}"/>
-    <hyperlink ref="B58" r:id="rId43" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805440976633856" xr:uid="{B6383852-5F85-4D3F-8B93-2865A580A285}"/>
-    <hyperlink ref="B104" r:id="rId44" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805439202443264" xr:uid="{FF314A10-1C40-49C4-89C4-9FE4279FC707}"/>
-    <hyperlink ref="B39" r:id="rId45" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805437411475456" xr:uid="{D08E76DB-B309-4B39-BE71-B80E22AE7EBF}"/>
-    <hyperlink ref="B98" r:id="rId46" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805435700199424" xr:uid="{9EA04559-C90F-4478-AC80-D97839D5F74C}"/>
-    <hyperlink ref="B147" r:id="rId47" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805433955368960" xr:uid="{F20CB891-5E97-4D09-B82D-85E97E8F4969}"/>
-    <hyperlink ref="B59" r:id="rId48" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805432256675840" xr:uid="{0CAC1D9E-7135-4583-9186-C8EB7A144268}"/>
-    <hyperlink ref="B51" r:id="rId49" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805430595731456" xr:uid="{2561C9C1-C311-4838-9090-9354D66F6FE6}"/>
-    <hyperlink ref="B53" r:id="rId50" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805429018673152" xr:uid="{3DF2B4DE-86F4-4350-98E5-6EF920DD91A5}"/>
-    <hyperlink ref="B18" r:id="rId51" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805427332562944" xr:uid="{2025E1AD-F296-4126-8299-D07CE8D76860}"/>
-    <hyperlink ref="B132" r:id="rId52" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805425780670464" xr:uid="{2ECB3326-0016-43DF-940C-BFF7ED76AEB6}"/>
-    <hyperlink ref="B30" r:id="rId53" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805424153280512" xr:uid="{545C7ACF-AF0F-47AB-90BD-438825FA0184}"/>
-    <hyperlink ref="B31" r:id="rId54" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805422639136768" xr:uid="{C286F0D9-2BDC-4BAC-8F03-D2739C5A2853}"/>
-    <hyperlink ref="B148" r:id="rId55" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805421066272768" xr:uid="{1DE3FC50-01F5-40DE-86F0-A31A5D76A2C3}"/>
-    <hyperlink ref="B23" r:id="rId56" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805419468242944" xr:uid="{7818A2D8-3ED5-46CB-A452-B4E51F6119D1}"/>
-    <hyperlink ref="B90" r:id="rId57" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805417945710592" xr:uid="{CBD25011-A015-4815-8F74-7345C69CF62C}"/>
-    <hyperlink ref="B47" r:id="rId58" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805416519647232" xr:uid="{716382A1-9D71-493C-AFB1-D6EE2945ADEB}"/>
-    <hyperlink ref="B73" r:id="rId59" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805415005503488" xr:uid="{B8EB85AF-A9FC-4408-8AA1-31228720C204}"/>
-    <hyperlink ref="B122" r:id="rId60" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805413520719872" xr:uid="{25FFB773-0778-463B-AC15-09EECD014643}"/>
-    <hyperlink ref="B129" r:id="rId61" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805411985604608" xr:uid="{0D925CF1-6AC7-4222-AAD4-D1B37454FE8E}"/>
-    <hyperlink ref="B69" r:id="rId62" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805410555346944" xr:uid="{145E67A0-E929-4C7B-8BAF-EE606CE525C4}"/>
-    <hyperlink ref="B44" r:id="rId63" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805409175420928" xr:uid="{900EDBED-C868-4014-BA1A-3B84214FF75B}"/>
-    <hyperlink ref="B4" r:id="rId64" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805407749357568" xr:uid="{65157475-2418-453C-990F-C2EAD997638B}"/>
+    <hyperlink ref="B34" r:id="rId33" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805458722734080" xr:uid="{9FE3426B-EE65-4BD4-82D5-4353808187B3}"/>
+    <hyperlink ref="B35" r:id="rId34" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805456881434624" xr:uid="{0BD5DC6A-5CF6-4859-BBDF-28DEE169D65C}"/>
+    <hyperlink ref="B36" r:id="rId35" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805454989803520" xr:uid="{3EF6CF64-9BE5-485E-915C-11254311497B}"/>
+    <hyperlink ref="B37" r:id="rId36" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805453203030016" xr:uid="{CEC48129-09DA-4BCD-8D86-EF37E2C8B021}"/>
+    <hyperlink ref="B38" r:id="rId37" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805451374313472" xr:uid="{8C7877FB-C53F-4C82-B693-8F3919AB588E}"/>
+    <hyperlink ref="B39" r:id="rId38" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805449625288704" xr:uid="{4C40021A-4B5F-49D8-953B-7B8BC23ACCE9}"/>
+    <hyperlink ref="B40" r:id="rId39" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805447855292416" xr:uid="{C07F5AB7-5FB1-4864-8D22-202836B5B8ED}"/>
+    <hyperlink ref="B41" r:id="rId40" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805446102073344" xr:uid="{A9A7264A-747F-48AE-82D8-302D31B349A1}"/>
+    <hyperlink ref="B42" r:id="rId41" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805444361437184" xr:uid="{3D1A5343-7724-4C55-AA9D-522F36978383}"/>
+    <hyperlink ref="B43" r:id="rId42" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805442671132672" xr:uid="{30B7B1A6-B7DF-41C8-A7FA-F624ABB35544}"/>
+    <hyperlink ref="B44" r:id="rId43" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805440976633856" xr:uid="{B6383852-5F85-4D3F-8B93-2865A580A285}"/>
+    <hyperlink ref="B45" r:id="rId44" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805439202443264" xr:uid="{FF314A10-1C40-49C4-89C4-9FE4279FC707}"/>
+    <hyperlink ref="B46" r:id="rId45" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805437411475456" xr:uid="{D08E76DB-B309-4B39-BE71-B80E22AE7EBF}"/>
+    <hyperlink ref="B47" r:id="rId46" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805435700199424" xr:uid="{9EA04559-C90F-4478-AC80-D97839D5F74C}"/>
+    <hyperlink ref="B48" r:id="rId47" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805433955368960" xr:uid="{F20CB891-5E97-4D09-B82D-85E97E8F4969}"/>
+    <hyperlink ref="B49" r:id="rId48" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805432256675840" xr:uid="{0CAC1D9E-7135-4583-9186-C8EB7A144268}"/>
+    <hyperlink ref="B50" r:id="rId49" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805430595731456" xr:uid="{2561C9C1-C311-4838-9090-9354D66F6FE6}"/>
+    <hyperlink ref="B51" r:id="rId50" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805429018673152" xr:uid="{3DF2B4DE-86F4-4350-98E5-6EF920DD91A5}"/>
+    <hyperlink ref="B52" r:id="rId51" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805427332562944" xr:uid="{2025E1AD-F296-4126-8299-D07CE8D76860}"/>
+    <hyperlink ref="B53" r:id="rId52" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805425780670464" xr:uid="{2ECB3326-0016-43DF-940C-BFF7ED76AEB6}"/>
+    <hyperlink ref="B55" r:id="rId53" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805424153280512" xr:uid="{545C7ACF-AF0F-47AB-90BD-438825FA0184}"/>
+    <hyperlink ref="B56" r:id="rId54" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805422639136768" xr:uid="{C286F0D9-2BDC-4BAC-8F03-D2739C5A2853}"/>
+    <hyperlink ref="B57" r:id="rId55" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805421066272768" xr:uid="{1DE3FC50-01F5-40DE-86F0-A31A5D76A2C3}"/>
+    <hyperlink ref="B58" r:id="rId56" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805419468242944" xr:uid="{7818A2D8-3ED5-46CB-A452-B4E51F6119D1}"/>
+    <hyperlink ref="B59" r:id="rId57" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805417945710592" xr:uid="{CBD25011-A015-4815-8F74-7345C69CF62C}"/>
+    <hyperlink ref="B60" r:id="rId58" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805416519647232" xr:uid="{716382A1-9D71-493C-AFB1-D6EE2945ADEB}"/>
+    <hyperlink ref="B61" r:id="rId59" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805415005503488" xr:uid="{B8EB85AF-A9FC-4408-8AA1-31228720C204}"/>
+    <hyperlink ref="B62" r:id="rId60" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805413520719872" xr:uid="{25FFB773-0778-463B-AC15-09EECD014643}"/>
+    <hyperlink ref="B63" r:id="rId61" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805411985604608" xr:uid="{0D925CF1-6AC7-4222-AAD4-D1B37454FE8E}"/>
+    <hyperlink ref="B64" r:id="rId62" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805410555346944" xr:uid="{145E67A0-E929-4C7B-8BAF-EE606CE525C4}"/>
+    <hyperlink ref="B65" r:id="rId63" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805409175420928" xr:uid="{900EDBED-C868-4014-BA1A-3B84214FF75B}"/>
+    <hyperlink ref="B66" r:id="rId64" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805407749357568" xr:uid="{65157475-2418-453C-990F-C2EAD997638B}"/>
     <hyperlink ref="B54" r:id="rId65" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805406352654336" xr:uid="{D8A3B0C2-27BF-4E49-A128-7FF617EBA77D}"/>
-    <hyperlink ref="B32" r:id="rId66" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805404939173888" xr:uid="{E9C31B62-A6D7-49FF-8FB6-6E2C15556CB0}"/>
-    <hyperlink ref="B91" r:id="rId67" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805403651522560" xr:uid="{CB221086-EB2A-475E-BC82-479E887CD859}"/>
-    <hyperlink ref="B99" r:id="rId68" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805402305150976" xr:uid="{A11FBA54-1D69-45F6-91EC-201BDD763B4A}"/>
-    <hyperlink ref="B61" r:id="rId69" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805400954585088" xr:uid="{8BA0B2E6-F600-418B-AD0A-56DA9FE26C53}"/>
-    <hyperlink ref="B78" r:id="rId70" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805399578853376" xr:uid="{6517B61F-1F01-4EAF-B07C-EE805688ABEE}"/>
-    <hyperlink ref="B67" r:id="rId71" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805398257647616" xr:uid="{89ADC396-21A1-4DFA-B40A-56C67E17AE65}"/>
-    <hyperlink ref="B105" r:id="rId72" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805396953219072" xr:uid="{80572BCD-509E-4CD2-A478-978EB496AD95}"/>
+    <hyperlink ref="B67" r:id="rId66" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805404939173888" xr:uid="{E9C31B62-A6D7-49FF-8FB6-6E2C15556CB0}"/>
+    <hyperlink ref="B68" r:id="rId67" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805403651522560" xr:uid="{CB221086-EB2A-475E-BC82-479E887CD859}"/>
+    <hyperlink ref="B69" r:id="rId68" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805402305150976" xr:uid="{A11FBA54-1D69-45F6-91EC-201BDD763B4A}"/>
+    <hyperlink ref="B70" r:id="rId69" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805400954585088" xr:uid="{8BA0B2E6-F600-418B-AD0A-56DA9FE26C53}"/>
+    <hyperlink ref="B71" r:id="rId70" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805399578853376" xr:uid="{6517B61F-1F01-4EAF-B07C-EE805688ABEE}"/>
+    <hyperlink ref="B72" r:id="rId71" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805398257647616" xr:uid="{89ADC396-21A1-4DFA-B40A-56C67E17AE65}"/>
+    <hyperlink ref="B73" r:id="rId72" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805396953219072" xr:uid="{80572BCD-509E-4CD2-A478-978EB496AD95}"/>
     <hyperlink ref="B74" r:id="rId73" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805395707510784" xr:uid="{7657AFB3-7266-416A-AC18-6F8529ECEE62}"/>
-    <hyperlink ref="B100" r:id="rId74" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805394512134144" xr:uid="{DF2040DF-0593-4753-9D4C-CC8BD7B34107}"/>
-    <hyperlink ref="B139" r:id="rId75" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805393241260032" xr:uid="{F359DCC5-4FA8-4043-B7C0-CD3277E344B8}"/>
-    <hyperlink ref="B48" r:id="rId76" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805392092020736" xr:uid="{08B6C803-56D6-410B-B71A-98B4BAA85931}"/>
-    <hyperlink ref="B141" r:id="rId77" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805390896644096" xr:uid="{737DE9A6-8ACB-460F-9CF4-117CBADC144E}"/>
-    <hyperlink ref="B114" r:id="rId78" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805389634158592" xr:uid="{B1AAD1F6-EABD-45CE-835D-14954FC05FF7}"/>
-    <hyperlink ref="B49" r:id="rId79" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805388447170560" xr:uid="{43995C04-EB4A-4F60-840C-F1713B7793F8}"/>
-    <hyperlink ref="B133" r:id="rId80" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805387268571136" xr:uid="{EB40D7AE-5F0A-4085-8413-A2C1A2FDFD4E}"/>
-    <hyperlink ref="B79" r:id="rId81" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805386161274880" xr:uid="{80F9CCAB-55EC-4A62-8072-9BEEDC29307A}"/>
-    <hyperlink ref="B106" r:id="rId82" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805385053978624" xr:uid="{20625644-B6B2-448A-BC10-72F47EC163B6}"/>
-    <hyperlink ref="B16" r:id="rId83" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805383929905152" xr:uid="{40688932-AF46-42F0-9CF8-9460A1E84287}"/>
-    <hyperlink ref="B35" r:id="rId84" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805382902300672" xr:uid="{E50F23EB-43BD-4C1F-9B8E-8AB8BEA8C7DF}"/>
-    <hyperlink ref="B115" r:id="rId85" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805381845336064" xr:uid="{33975410-0C8A-42EF-A765-3A6999E3CC60}"/>
-    <hyperlink ref="B28" r:id="rId86" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805380754817024" xr:uid="{BE6A4AEE-2B81-4711-93A5-31AB11DE59E0}"/>
-    <hyperlink ref="B36" r:id="rId87" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805379664297984" xr:uid="{64DBE82A-9F48-4162-8ABC-12AB42900515}"/>
-    <hyperlink ref="B80" r:id="rId88" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805378443755520" xr:uid="{F3651311-CE8A-4594-BF9A-F62D8CF784CE}"/>
-    <hyperlink ref="B55" r:id="rId89" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805377432928256" xr:uid="{DD9E91A5-4CD7-46F9-B7C1-32FF0A6F23B5}"/>
-    <hyperlink ref="B62" r:id="rId90" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805376476626944" xr:uid="{91829DBE-D577-4BB1-82FF-7396B01788B3}"/>
-    <hyperlink ref="B101" r:id="rId91" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805375457411072" xr:uid="{A6880981-AB8A-4EAD-9CAD-264502E6DE7A}"/>
-    <hyperlink ref="B29" r:id="rId92" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805374509498368" xr:uid="{30436A1D-7844-485C-9B25-2FA7ED82ACE2}"/>
-    <hyperlink ref="B81" r:id="rId93" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805373582557184" xr:uid="{C986EBF0-E06F-4D2A-9853-6DC592F7D5DC}"/>
-    <hyperlink ref="B8" r:id="rId94" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805372601090048" xr:uid="{3C48E432-2B14-4FB2-BAA5-4D5B4E447A5C}"/>
-    <hyperlink ref="B137" r:id="rId95" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805371602845696" xr:uid="{1F092979-C59D-474B-BE78-A133D8C3F3E5}"/>
-    <hyperlink ref="B83" r:id="rId96" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805370650738688" xr:uid="{EF850CE3-4899-49A8-9BB4-2591BC7D81D9}"/>
-    <hyperlink ref="B84" r:id="rId97" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805369774129152" xr:uid="{668DE3E3-CC71-4E3E-9A8D-015F2792011D}"/>
-    <hyperlink ref="B63" r:id="rId98" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805368847187968" xr:uid="{01A62861-3DC4-431D-8433-195661815291}"/>
-    <hyperlink ref="B5" r:id="rId99" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805367987355648" xr:uid="{8FE03253-9901-4CB2-B1EC-C2EB483D2377}"/>
-    <hyperlink ref="B85" r:id="rId100" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805367156883456" xr:uid="{E6326954-D001-497F-BC5E-05BB9994247D}"/>
-    <hyperlink ref="B123" r:id="rId101" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805366343188480" xr:uid="{9B63539D-ABF1-43A0-ADC2-06B118D72D66}"/>
-    <hyperlink ref="B14" r:id="rId102" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805365537882112" xr:uid="{49162591-2FC2-44DA-9BF4-CB80606B71AC}"/>
-    <hyperlink ref="B82" r:id="rId103" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805364711604224" xr:uid="{0F71C7FB-9FAC-4882-894C-A0CE8C6A5985}"/>
-    <hyperlink ref="B75" r:id="rId104" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805363914686464" xr:uid="{520DAE34-44B4-4BFF-B556-43A2E602BC27}"/>
-    <hyperlink ref="B68" r:id="rId105" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805363117768704" xr:uid="{E6CE24ED-637E-4FC3-962F-BF33DDA343B1}"/>
-    <hyperlink ref="B40" r:id="rId106" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805362341822464" xr:uid="{8E6583D9-83BE-4AAA-919E-7E9073C8734F}"/>
-    <hyperlink ref="B64" r:id="rId107" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805361586847744" xr:uid="{27689A09-DC7F-4850-AD4D-4A4EA6113611}"/>
-    <hyperlink ref="B108" r:id="rId108" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805360777347072" xr:uid="{25D61D27-A5F4-4BA8-ADBE-8A94C62B56B3}"/>
-    <hyperlink ref="B56" r:id="rId109" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805360043343872" xr:uid="{728FA30F-1439-4A82-BC48-3A177A9436AE}"/>
-    <hyperlink ref="B92" r:id="rId110" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805359372255232" xr:uid="{549016E0-2188-4FA9-9DF2-285C4CB5F6E4}"/>
-    <hyperlink ref="B130" r:id="rId111" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805358663417856" xr:uid="{A089EAA5-6EA0-4290-8ACC-6261DA94AD9F}"/>
-    <hyperlink ref="B119" r:id="rId112" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805357933608960" xr:uid="{6B9BB080-9DD3-4124-957B-5E38F6A2526F}"/>
+    <hyperlink ref="B75" r:id="rId74" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805394512134144" xr:uid="{DF2040DF-0593-4753-9D4C-CC8BD7B34107}"/>
+    <hyperlink ref="B76" r:id="rId75" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805393241260032" xr:uid="{F359DCC5-4FA8-4043-B7C0-CD3277E344B8}"/>
+    <hyperlink ref="B77" r:id="rId76" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805392092020736" xr:uid="{08B6C803-56D6-410B-B71A-98B4BAA85931}"/>
+    <hyperlink ref="B78" r:id="rId77" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805390896644096" xr:uid="{737DE9A6-8ACB-460F-9CF4-117CBADC144E}"/>
+    <hyperlink ref="B79" r:id="rId78" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805389634158592" xr:uid="{B1AAD1F6-EABD-45CE-835D-14954FC05FF7}"/>
+    <hyperlink ref="B80" r:id="rId79" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805388447170560" xr:uid="{43995C04-EB4A-4F60-840C-F1713B7793F8}"/>
+    <hyperlink ref="B81" r:id="rId80" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805387268571136" xr:uid="{EB40D7AE-5F0A-4085-8413-A2C1A2FDFD4E}"/>
+    <hyperlink ref="B82" r:id="rId81" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805386161274880" xr:uid="{80F9CCAB-55EC-4A62-8072-9BEEDC29307A}"/>
+    <hyperlink ref="B83" r:id="rId82" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805385053978624" xr:uid="{20625644-B6B2-448A-BC10-72F47EC163B6}"/>
+    <hyperlink ref="B84" r:id="rId83" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805383929905152" xr:uid="{40688932-AF46-42F0-9CF8-9460A1E84287}"/>
+    <hyperlink ref="B85" r:id="rId84" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805382902300672" xr:uid="{E50F23EB-43BD-4C1F-9B8E-8AB8BEA8C7DF}"/>
+    <hyperlink ref="B86" r:id="rId85" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805381845336064" xr:uid="{33975410-0C8A-42EF-A765-3A6999E3CC60}"/>
+    <hyperlink ref="B87" r:id="rId86" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805380754817024" xr:uid="{BE6A4AEE-2B81-4711-93A5-31AB11DE59E0}"/>
+    <hyperlink ref="B88" r:id="rId87" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805379664297984" xr:uid="{64DBE82A-9F48-4162-8ABC-12AB42900515}"/>
+    <hyperlink ref="B89" r:id="rId88" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805378443755520" xr:uid="{F3651311-CE8A-4594-BF9A-F62D8CF784CE}"/>
+    <hyperlink ref="B90" r:id="rId89" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805377432928256" xr:uid="{DD9E91A5-4CD7-46F9-B7C1-32FF0A6F23B5}"/>
+    <hyperlink ref="B91" r:id="rId90" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805376476626944" xr:uid="{91829DBE-D577-4BB1-82FF-7396B01788B3}"/>
+    <hyperlink ref="B92" r:id="rId91" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805375457411072" xr:uid="{A6880981-AB8A-4EAD-9CAD-264502E6DE7A}"/>
+    <hyperlink ref="B93" r:id="rId92" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805374509498368" xr:uid="{30436A1D-7844-485C-9B25-2FA7ED82ACE2}"/>
+    <hyperlink ref="B94" r:id="rId93" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805373582557184" xr:uid="{C986EBF0-E06F-4D2A-9853-6DC592F7D5DC}"/>
+    <hyperlink ref="B95" r:id="rId94" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805372601090048" xr:uid="{3C48E432-2B14-4FB2-BAA5-4D5B4E447A5C}"/>
+    <hyperlink ref="B96" r:id="rId95" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805371602845696" xr:uid="{1F092979-C59D-474B-BE78-A133D8C3F3E5}"/>
+    <hyperlink ref="B97" r:id="rId96" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805370650738688" xr:uid="{EF850CE3-4899-49A8-9BB4-2591BC7D81D9}"/>
+    <hyperlink ref="B98" r:id="rId97" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805369774129152" xr:uid="{668DE3E3-CC71-4E3E-9A8D-015F2792011D}"/>
+    <hyperlink ref="B99" r:id="rId98" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805368847187968" xr:uid="{01A62861-3DC4-431D-8433-195661815291}"/>
+    <hyperlink ref="B100" r:id="rId99" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805367987355648" xr:uid="{8FE03253-9901-4CB2-B1EC-C2EB483D2377}"/>
+    <hyperlink ref="B101" r:id="rId100" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805367156883456" xr:uid="{E6326954-D001-497F-BC5E-05BB9994247D}"/>
+    <hyperlink ref="B102" r:id="rId101" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805366343188480" xr:uid="{9B63539D-ABF1-43A0-ADC2-06B118D72D66}"/>
+    <hyperlink ref="B103" r:id="rId102" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805365537882112" xr:uid="{49162591-2FC2-44DA-9BF4-CB80606B71AC}"/>
+    <hyperlink ref="B104" r:id="rId103" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805364711604224" xr:uid="{0F71C7FB-9FAC-4882-894C-A0CE8C6A5985}"/>
+    <hyperlink ref="B105" r:id="rId104" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805363914686464" xr:uid="{520DAE34-44B4-4BFF-B556-43A2E602BC27}"/>
+    <hyperlink ref="B106" r:id="rId105" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805363117768704" xr:uid="{E6CE24ED-637E-4FC3-962F-BF33DDA343B1}"/>
+    <hyperlink ref="B108" r:id="rId106" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805362341822464" xr:uid="{8E6583D9-83BE-4AAA-919E-7E9073C8734F}"/>
+    <hyperlink ref="B109" r:id="rId107" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805361586847744" xr:uid="{27689A09-DC7F-4850-AD4D-4A4EA6113611}"/>
+    <hyperlink ref="B110" r:id="rId108" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805360777347072" xr:uid="{25D61D27-A5F4-4BA8-ADBE-8A94C62B56B3}"/>
+    <hyperlink ref="B111" r:id="rId109" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805360043343872" xr:uid="{728FA30F-1439-4A82-BC48-3A177A9436AE}"/>
+    <hyperlink ref="B112" r:id="rId110" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805359372255232" xr:uid="{549016E0-2188-4FA9-9DF2-285C4CB5F6E4}"/>
+    <hyperlink ref="B113" r:id="rId111" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805358663417856" xr:uid="{A089EAA5-6EA0-4290-8ACC-6261DA94AD9F}"/>
+    <hyperlink ref="B114" r:id="rId112" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805357933608960" xr:uid="{6B9BB080-9DD3-4124-957B-5E38F6A2526F}"/>
     <hyperlink ref="B107" r:id="rId113" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805357258326016" xr:uid="{5FFC3AC7-208A-4DDA-B956-1446DF73288C}"/>
-    <hyperlink ref="B19" r:id="rId114" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805356599820288" xr:uid="{D061F457-D3B3-4DEA-9415-95F3A6571951}"/>
-    <hyperlink ref="B37" r:id="rId115" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805355987451904" xr:uid="{19C7365A-379D-4B72-BA1B-4EBA50FBCB4D}"/>
-    <hyperlink ref="B45" r:id="rId116" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805355358306304" xr:uid="{E7AAE68F-15B1-43EB-A3AF-B3711F97E3CA}"/>
-    <hyperlink ref="B109" r:id="rId117" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805354762715136" xr:uid="{CC85E1B5-8D6C-443E-A353-3901DB444CE5}"/>
-    <hyperlink ref="B102" r:id="rId118" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805354108403712" xr:uid="{D2DEA07B-B9E6-46E3-BF41-52465EA6A993}"/>
-    <hyperlink ref="B144" r:id="rId119" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805353470869504" xr:uid="{F712684E-8D42-446C-A76F-C503C11D0D47}"/>
+    <hyperlink ref="B115" r:id="rId114" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805356599820288" xr:uid="{D061F457-D3B3-4DEA-9415-95F3A6571951}"/>
+    <hyperlink ref="B116" r:id="rId115" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805355987451904" xr:uid="{19C7365A-379D-4B72-BA1B-4EBA50FBCB4D}"/>
+    <hyperlink ref="B117" r:id="rId116" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805355358306304" xr:uid="{E7AAE68F-15B1-43EB-A3AF-B3711F97E3CA}"/>
+    <hyperlink ref="B119" r:id="rId117" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805354762715136" xr:uid="{CC85E1B5-8D6C-443E-A353-3901DB444CE5}"/>
+    <hyperlink ref="B120" r:id="rId118" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805354108403712" xr:uid="{D2DEA07B-B9E6-46E3-BF41-52465EA6A993}"/>
+    <hyperlink ref="B121" r:id="rId119" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805353470869504" xr:uid="{F712684E-8D42-446C-A76F-C503C11D0D47}"/>
     <hyperlink ref="B118" r:id="rId120" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805352925609984" xr:uid="{4885942E-8962-4648-9202-4753000FD40B}"/>
-    <hyperlink ref="B65" r:id="rId121" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805352359378944" xr:uid="{02011A0F-B669-4EAB-8A70-878E94ACDA37}"/>
-    <hyperlink ref="B41" r:id="rId122" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805351814119424" xr:uid="{45A708F0-933E-4855-9B5E-244E61913E7C}"/>
-    <hyperlink ref="B13" r:id="rId123" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805351302414336" xr:uid="{572E398C-087F-49D6-9BE2-612B34EFFAED}"/>
-    <hyperlink ref="B42" r:id="rId124" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805350803292160" xr:uid="{7F77C1E2-8F2E-4438-9C7C-96805716246F}"/>
-    <hyperlink ref="B10" r:id="rId125" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805350316752896" xr:uid="{66389BD4-0069-4C78-BA84-A177C9D1D4EA}"/>
-    <hyperlink ref="B124" r:id="rId126" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805349851185152" xr:uid="{6CBA2366-28A4-46AA-92BD-D6AD9A5FE8AE}"/>
-    <hyperlink ref="B9" r:id="rId127" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805349394006016" xr:uid="{7768D139-E482-4930-BBD0-E823226E364D}"/>
-    <hyperlink ref="B57" r:id="rId128" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805348915855360" xr:uid="{41B57192-5CDB-46F1-B822-78C81C2124A4}"/>
-    <hyperlink ref="B76" r:id="rId129" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805348471259136" xr:uid="{DFF5C9CF-700C-4097-A4C7-619CCC48FD60}"/>
-    <hyperlink ref="B20" r:id="rId130" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805347921805312" xr:uid="{3B0E82D2-99C9-48AF-ADFD-8BD03A59A824}"/>
-    <hyperlink ref="B134" r:id="rId131" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805347523346432" xr:uid="{44D51ACD-CFC3-47A4-8A79-39811F3ADA11}"/>
-    <hyperlink ref="B77" r:id="rId132" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805347145859072" xr:uid="{0E26BABB-1220-42C1-834C-CA692D69862D}"/>
-    <hyperlink ref="B86" r:id="rId133" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805346776760320" xr:uid="{EE955F28-4376-4D9C-AB3D-ED90FE8A39F2}"/>
-    <hyperlink ref="B17" r:id="rId134" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805346428633088" xr:uid="{6E4BFF91-3893-4AA2-B7DC-095978898326}"/>
-    <hyperlink ref="B120" r:id="rId135" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805346063728640" xr:uid="{05AE5EF5-1080-47C7-A4BB-5987FD51B2B3}"/>
-    <hyperlink ref="B93" r:id="rId136" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805345732378624" xr:uid="{AB415585-E55B-4374-B536-4C4856168D81}"/>
-    <hyperlink ref="B110" r:id="rId137" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805345401028608" xr:uid="{5B316447-8B80-4D38-9E5B-B88CF9A8D7AA}"/>
-    <hyperlink ref="B116" r:id="rId138" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805345078067200" xr:uid="{3C202DED-461A-4080-AA72-3D2F06C11EB7}"/>
-    <hyperlink ref="B143" r:id="rId139" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805344776077312" xr:uid="{8973E54D-8116-4D12-9F6B-A908718A0C94}"/>
-    <hyperlink ref="B70" r:id="rId140" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805344490864640" xr:uid="{95E29B44-90F9-491C-A72D-13224B7FD39E}"/>
+    <hyperlink ref="B122" r:id="rId121" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805352359378944" xr:uid="{02011A0F-B669-4EAB-8A70-878E94ACDA37}"/>
+    <hyperlink ref="B123" r:id="rId122" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805351814119424" xr:uid="{45A708F0-933E-4855-9B5E-244E61913E7C}"/>
+    <hyperlink ref="B124" r:id="rId123" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805351302414336" xr:uid="{572E398C-087F-49D6-9BE2-612B34EFFAED}"/>
+    <hyperlink ref="B125" r:id="rId124" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805350803292160" xr:uid="{7F77C1E2-8F2E-4438-9C7C-96805716246F}"/>
+    <hyperlink ref="B126" r:id="rId125" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805350316752896" xr:uid="{66389BD4-0069-4C78-BA84-A177C9D1D4EA}"/>
+    <hyperlink ref="B127" r:id="rId126" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805349851185152" xr:uid="{6CBA2366-28A4-46AA-92BD-D6AD9A5FE8AE}"/>
+    <hyperlink ref="B128" r:id="rId127" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805349394006016" xr:uid="{7768D139-E482-4930-BBD0-E823226E364D}"/>
+    <hyperlink ref="B129" r:id="rId128" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805348915855360" xr:uid="{41B57192-5CDB-46F1-B822-78C81C2124A4}"/>
+    <hyperlink ref="B130" r:id="rId129" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805348471259136" xr:uid="{DFF5C9CF-700C-4097-A4C7-619CCC48FD60}"/>
+    <hyperlink ref="B131" r:id="rId130" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805347921805312" xr:uid="{3B0E82D2-99C9-48AF-ADFD-8BD03A59A824}"/>
+    <hyperlink ref="B132" r:id="rId131" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805347523346432" xr:uid="{44D51ACD-CFC3-47A4-8A79-39811F3ADA11}"/>
+    <hyperlink ref="B133" r:id="rId132" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805347145859072" xr:uid="{0E26BABB-1220-42C1-834C-CA692D69862D}"/>
+    <hyperlink ref="B134" r:id="rId133" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805346776760320" xr:uid="{EE955F28-4376-4D9C-AB3D-ED90FE8A39F2}"/>
+    <hyperlink ref="B135" r:id="rId134" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805346428633088" xr:uid="{6E4BFF91-3893-4AA2-B7DC-095978898326}"/>
+    <hyperlink ref="B136" r:id="rId135" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805346063728640" xr:uid="{05AE5EF5-1080-47C7-A4BB-5987FD51B2B3}"/>
+    <hyperlink ref="B137" r:id="rId136" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805345732378624" xr:uid="{AB415585-E55B-4374-B536-4C4856168D81}"/>
+    <hyperlink ref="B138" r:id="rId137" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805345401028608" xr:uid="{5B316447-8B80-4D38-9E5B-B88CF9A8D7AA}"/>
+    <hyperlink ref="B139" r:id="rId138" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805345078067200" xr:uid="{3C202DED-461A-4080-AA72-3D2F06C11EB7}"/>
+    <hyperlink ref="B140" r:id="rId139" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805344776077312" xr:uid="{8973E54D-8116-4D12-9F6B-A908718A0C94}"/>
+    <hyperlink ref="B141" r:id="rId140" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805344490864640" xr:uid="{95E29B44-90F9-491C-A72D-13224B7FD39E}"/>
     <hyperlink ref="B142" r:id="rId141" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805344222429184" xr:uid="{EEA8E464-998C-4619-98C9-AFA2714C8DD9}"/>
-    <hyperlink ref="B34" r:id="rId142" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343979159552" xr:uid="{6B730A56-AD16-4ADC-8C63-B162926E9F92}"/>
-    <hyperlink ref="B125" r:id="rId143" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343727501312" xr:uid="{5B17F22B-97FD-4A77-A01A-8C86EACC527F}"/>
-    <hyperlink ref="B131" r:id="rId144" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343463260160" xr:uid="{5D59B2A4-4BD8-4DD2-B31C-EA0CEF2A6105}"/>
-    <hyperlink ref="B126" r:id="rId145" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343236767744" xr:uid="{4E9CFC68-DF13-4062-92B9-8586049818CD}"/>
-    <hyperlink ref="B38" r:id="rId146" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343043829760" xr:uid="{6B0ED80C-8D5E-44DB-9A3D-61DD2A698EEB}"/>
-    <hyperlink ref="B94" r:id="rId147" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805342821531648" xr:uid="{F5F0C8F2-C2C8-4576-A386-FE0A8EA6D75A}"/>
+    <hyperlink ref="B143" r:id="rId142" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343979159552" xr:uid="{6B730A56-AD16-4ADC-8C63-B162926E9F92}"/>
+    <hyperlink ref="B144" r:id="rId143" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343727501312" xr:uid="{5B17F22B-97FD-4A77-A01A-8C86EACC527F}"/>
+    <hyperlink ref="B145" r:id="rId144" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343463260160" xr:uid="{5D59B2A4-4BD8-4DD2-B31C-EA0CEF2A6105}"/>
+    <hyperlink ref="B146" r:id="rId145" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343236767744" xr:uid="{4E9CFC68-DF13-4062-92B9-8586049818CD}"/>
+    <hyperlink ref="B147" r:id="rId146" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805343043829760" xr:uid="{6B0ED80C-8D5E-44DB-9A3D-61DD2A698EEB}"/>
+    <hyperlink ref="B148" r:id="rId147" display="https://pintia.cn/problem-sets/994805342720868352/problems/994805342821531648" xr:uid="{F5F0C8F2-C2C8-4576-A386-FE0A8EA6D75A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId148"/>

</xml_diff>

<commit_message>
first commit 1097(Python) 1097 Deduplication on a Linked List (25) 部分正确	13	1097	Python (python 3)	24 ms
</commit_message>
<xml_diff>
--- a/PAT-Advanced-Level-Practice.xlsx
+++ b/PAT-Advanced-Level-Practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\hp_WJ\Documents\GitHub\PAT-Advanced-Level-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF0F9AB8-A208-41BE-8AF6-485AD084A7EA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FD6CFC9-D231-43F5-A019-DD6109619EE4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9612" xr2:uid="{B69768DD-3D21-489D-9183-877BD9BED12D}"/>
   </bookViews>
@@ -937,8 +937,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I70" sqref="I70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2473,7 +2473,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>1074</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>1097</v>
       </c>
@@ -2954,6 +2954,9 @@
       </c>
       <c r="F98" s="4">
         <v>0.3</v>
+      </c>
+      <c r="G98" s="2">
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
2018年8月11日日志 修改 1074(Python) 1074 Reversing Linked List (25) 部分正确	22	1074	Python (python 3) 更改部分文件的名字
</commit_message>
<xml_diff>
--- a/PAT-Advanced-Level-Practice.xlsx
+++ b/PAT-Advanced-Level-Practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\hp_WJ\Documents\GitHub\PAT-Advanced-Level-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FD6CFC9-D231-43F5-A019-DD6109619EE4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{02146693-BA27-420F-B795-9E26792E9CDE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9612" xr2:uid="{B69768DD-3D21-489D-9183-877BD9BED12D}"/>
   </bookViews>
@@ -938,7 +938,7 @@
   <dimension ref="A1:G148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2493,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G75" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3971,7 +3971,7 @@
       <filters blank="1"/>
     </filterColumn>
     <sortState ref="A4:G148">
-      <sortCondition ref="A1:A148"/>
+      <sortCondition ref="G1:G148"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
2018年8月13日日志 1、首次提交 1009(Python) 1009 Product of Polynomials (25) 部分正确	15	1009	Python (python 3)	26 ms 2、更新部分文件
</commit_message>
<xml_diff>
--- a/PAT-Advanced-Level-Practice.xlsx
+++ b/PAT-Advanced-Level-Practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\hp_WJ\Documents\GitHub\PAT-Advanced-Level-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{02146693-BA27-420F-B795-9E26792E9CDE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{44041008-6F71-4634-9F45-603EF3386EA8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9612" xr2:uid="{B69768DD-3D21-489D-9183-877BD9BED12D}"/>
   </bookViews>
@@ -938,7 +938,7 @@
   <dimension ref="A1:G148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1141,6 +1141,9 @@
       </c>
       <c r="F9" s="4">
         <v>0.28000000000000003</v>
+      </c>
+      <c r="G9" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
2018年8月17日日志 1、首次提交 1015(C++) 1015 Reversible Primes (20) 答案正确	20	1015	C++ (g++)	3 ms 2、更新部分文件 祝七夕节快乐
</commit_message>
<xml_diff>
--- a/PAT-Advanced-Level-Practice.xlsx
+++ b/PAT-Advanced-Level-Practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\hp_WJ\Documents\GitHub\PAT-Advanced-Level-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{44041008-6F71-4634-9F45-603EF3386EA8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{69F88CD9-6C5D-414D-9C1D-122D8F5BBCB7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9612" xr2:uid="{B69768DD-3D21-489D-9183-877BD9BED12D}"/>
   </bookViews>
@@ -938,7 +938,7 @@
   <dimension ref="A1:G148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1123,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1009</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="19.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1015</v>
       </c>
@@ -1293,6 +1293,9 @@
       </c>
       <c r="F16" s="4">
         <v>0.28000000000000003</v>
+      </c>
+      <c r="G16" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2496,7 +2499,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G75" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>